<commit_message>
Code ver. 2.1  26-feb-15
26-feb-15

Error Handlers added. (Updated PI and PC versions of sx4)

Updated db.py for PI version

Removed extra db,sx4,tst versions from folder.

tst.py updated for PC version >>>>   # axes = adxl345.getAxes(True)
</commit_message>
<xml_diff>
--- a/Code/SX4 SUPPORTED PIDs.xlsx
+++ b/Code/SX4 SUPPORTED PIDs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="118">
   <si>
     <t>A*100/255</t>
   </si>
@@ -726,24 +726,24 @@
   <dimension ref="A1:DW34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="36.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="12.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="38.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="27.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="36.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="2"/>
+    <col min="7" max="7" width="12.44140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="38.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="27.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:127" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:127" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -792,7 +792,7 @@
       <c r="DO1" s="1"/>
       <c r="DW1" s="1"/>
     </row>
-    <row r="3" spans="1:127" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:127" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -815,13 +815,16 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:127" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:127" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>44</v>
       </c>
+      <c r="C4" t="s">
+        <v>116</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
@@ -838,7 +841,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:127" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:127" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -861,7 +864,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:127" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:127" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -884,7 +887,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:127" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:127" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -907,7 +910,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:127" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:127" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -918,7 +921,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:127" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:127" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -941,7 +944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:127" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:127" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -967,7 +970,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:127" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:127" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -993,7 +996,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:127" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:127" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1019,7 +1022,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:127" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:127" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -1045,7 +1048,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:127" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:127" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
@@ -1071,7 +1074,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:127" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:127" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
@@ -1097,7 +1100,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -1123,7 +1126,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
@@ -1149,7 +1152,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>28</v>
       </c>
@@ -1175,7 +1178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>30</v>
       </c>
@@ -1216,7 +1219,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
@@ -1257,7 +1260,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
@@ -1283,7 +1286,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>31</v>
       </c>
@@ -1309,7 +1312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>33</v>
       </c>
@@ -1335,7 +1338,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>34</v>
       </c>
@@ -1361,7 +1364,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>35</v>
       </c>
@@ -1387,7 +1390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>36</v>
       </c>
@@ -1413,7 +1416,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>37</v>
       </c>
@@ -1439,7 +1442,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>38</v>
       </c>
@@ -1465,7 +1468,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>39</v>
       </c>
@@ -1491,7 +1494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>40</v>
       </c>
@@ -1517,7 +1520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>41</v>
       </c>
@@ -1543,7 +1546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>42</v>
       </c>
@@ -1569,7 +1572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>43</v>
       </c>
@@ -1610,7 +1613,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1622,7 +1625,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>